<commit_message>
update data provider to use arraylist and maps
</commit_message>
<xml_diff>
--- a/src/test/test-resources/TestData.xlsx
+++ b/src/test/test-resources/TestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
   <si>
     <t xml:space="preserve">Smoke</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t xml:space="preserve">02/28/1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMITH1</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
@@ -461,7 +467,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -502,11 +508,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -917,10 +919,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,14 +933,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.58"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -966,19 +968,19 @@
       <c r="I1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -992,7 +994,7 @@
       <c r="C2" s="1" t="n">
         <v>362</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="10" t="n">
         <v>12013514000</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1010,25 +1012,70 @@
       <c r="I2" s="1" t="n">
         <v>30318</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>9800</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
+        <v>112223333</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>12013514000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>30318</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>9800</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="1" t="n">
         <v>112223333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="kbisht@lendingpoint.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="kbisht@lendingpoint.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1072,31 +1119,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>57</v>
@@ -1108,154 +1155,154 @@
         <v>59</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>101</v>
       </c>
+      <c r="N2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="O3" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="K4" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="M4" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="N4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>